<commit_message>
Updated way of calculating initial prop
</commit_message>
<xml_diff>
--- a/results/ResultsTableAndGraphs.xlsx
+++ b/results/ResultsTableAndGraphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -221,31 +221,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.63129999999999997</c:v>
+                  <c:v>0.61339999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.745</c:v>
+                  <c:v>0.71260000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83530000000000004</c:v>
+                  <c:v>0.82769999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89039999999999997</c:v>
+                  <c:v>0.87180000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.89039999999999997</c:v>
+                  <c:v>0.87250000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.87529999999999997</c:v>
+                  <c:v>0.82840000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.87529999999999997</c:v>
+                  <c:v>0.85729999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.90759999999999996</c:v>
+                  <c:v>0.88970000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.92420000000000002</c:v>
+                  <c:v>0.90559999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -290,31 +290,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.76910000000000001</c:v>
+                  <c:v>0.7954</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76670000000000005</c:v>
+                  <c:v>0.78690000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77490000000000003</c:v>
+                  <c:v>0.79849999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75380000000000003</c:v>
+                  <c:v>0.78620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.76129999999999998</c:v>
+                  <c:v>0.78879999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75419999999999998</c:v>
+                  <c:v>0.77849999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75370000000000004</c:v>
+                  <c:v>0.78090000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76219999999999999</c:v>
+                  <c:v>0.78910000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.75460000000000005</c:v>
+                  <c:v>0.78590000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,31 +359,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.60370000000000001</c:v>
+                  <c:v>0.61040000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67079999999999995</c:v>
+                  <c:v>0.66590000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73180000000000001</c:v>
+                  <c:v>0.74509999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.74880000000000002</c:v>
+                  <c:v>0.76290000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.75490000000000002</c:v>
+                  <c:v>0.76529999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7399</c:v>
+                  <c:v>0.73040000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73950000000000005</c:v>
+                  <c:v>0.74990000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7661</c:v>
+                  <c:v>0.77629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77010000000000001</c:v>
+                  <c:v>0.78359999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,7 +412,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -428,31 +428,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.60509999999999997</c:v>
+                  <c:v>0.61299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67090000000000005</c:v>
+                  <c:v>0.66620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73199999999999998</c:v>
+                  <c:v>0.74509999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.74980000000000002</c:v>
+                  <c:v>0.76329999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.75570000000000004</c:v>
+                  <c:v>0.76570000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.74070000000000003</c:v>
+                  <c:v>0.73050000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.74029999999999996</c:v>
+                  <c:v>0.75029999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7671</c:v>
+                  <c:v>0.77680000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77149999999999996</c:v>
+                  <c:v>0.7843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -767,22 +767,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.61270000000000002</c:v>
+                  <c:v>0.56030000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7298</c:v>
+                  <c:v>0.71189999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.80010000000000003</c:v>
+                  <c:v>0.79259999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89319999999999999</c:v>
+                  <c:v>0.90349999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86699999999999999</c:v>
+                  <c:v>0.84909999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.86699999999999999</c:v>
+                  <c:v>0.84909999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.88149999999999995</c:v>
@@ -791,7 +791,7 @@
                   <c:v>0.89459999999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.89870000000000005</c:v>
+                  <c:v>0.89590000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -820,7 +820,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -836,31 +836,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.75600000000000001</c:v>
+                  <c:v>0.78549999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77580000000000005</c:v>
+                  <c:v>0.79890000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.79849999999999999</c:v>
+                  <c:v>0.82499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.77049999999999996</c:v>
+                  <c:v>0.80330000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.77749999999999997</c:v>
+                  <c:v>0.80420000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.77649999999999997</c:v>
+                  <c:v>0.7923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.77139999999999997</c:v>
+                  <c:v>0.79890000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76800000000000002</c:v>
+                  <c:v>0.78859999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77849999999999997</c:v>
+                  <c:v>0.80300000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,31 +905,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.58330000000000004</c:v>
+                  <c:v>0.57079999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66839999999999999</c:v>
+                  <c:v>0.67400000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.72799999999999998</c:v>
+                  <c:v>0.74260000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76380000000000003</c:v>
+                  <c:v>0.79579999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.75319999999999998</c:v>
+                  <c:v>0.76249999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75249999999999995</c:v>
+                  <c:v>0.75360000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75729999999999997</c:v>
+                  <c:v>0.77859999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76270000000000004</c:v>
+                  <c:v>0.77880000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77349999999999997</c:v>
+                  <c:v>0.79079999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,31 +974,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.58489999999999998</c:v>
+                  <c:v>0.57499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66849999999999998</c:v>
+                  <c:v>0.67449999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.72799999999999998</c:v>
+                  <c:v>0.74270000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76459999999999995</c:v>
+                  <c:v>0.79630000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.76270000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.75370000000000004</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.752</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75800000000000001</c:v>
+                  <c:v>0.77900000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76349999999999996</c:v>
+                  <c:v>0.77939999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.7742</c:v>
+                  <c:v>0.79120000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2322,15 +2322,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>140493</xdr:colOff>
+      <xdr:colOff>140492</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>92870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>61914</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>595313</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2358,15 +2358,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>611980</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>21432</xdr:rowOff>
+      <xdr:colOff>540543</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>140494</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>157163</xdr:rowOff>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2691,10 +2691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2729,16 +2729,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0.63129999999999997</v>
+        <v>0.61339999999999995</v>
       </c>
       <c r="C4">
-        <v>0.76910000000000001</v>
+        <v>0.7954</v>
       </c>
       <c r="D4">
-        <v>0.60370000000000001</v>
+        <v>0.61040000000000005</v>
       </c>
       <c r="E4">
-        <v>0.60509999999999997</v>
+        <v>0.61299999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -2746,16 +2746,16 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0.745</v>
+        <v>0.71260000000000001</v>
       </c>
       <c r="C5">
-        <v>0.76670000000000005</v>
+        <v>0.78690000000000004</v>
       </c>
       <c r="D5">
-        <v>0.67079999999999995</v>
+        <v>0.66590000000000005</v>
       </c>
       <c r="E5">
-        <v>0.67090000000000005</v>
+        <v>0.66620000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -2763,16 +2763,16 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>0.83530000000000004</v>
+        <v>0.82769999999999999</v>
       </c>
       <c r="C6">
-        <v>0.77490000000000003</v>
+        <v>0.79849999999999999</v>
       </c>
       <c r="D6">
-        <v>0.73180000000000001</v>
+        <v>0.74509999999999998</v>
       </c>
       <c r="E6">
-        <v>0.73199999999999998</v>
+        <v>0.74509999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -2780,16 +2780,16 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>0.89039999999999997</v>
+        <v>0.87180000000000002</v>
       </c>
       <c r="C7">
-        <v>0.75380000000000003</v>
+        <v>0.78620000000000001</v>
       </c>
       <c r="D7">
-        <v>0.74880000000000002</v>
+        <v>0.76290000000000002</v>
       </c>
       <c r="E7">
-        <v>0.74980000000000002</v>
+        <v>0.76329999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -2797,16 +2797,16 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0.89039999999999997</v>
+        <v>0.87250000000000005</v>
       </c>
       <c r="C8">
-        <v>0.76129999999999998</v>
+        <v>0.78879999999999995</v>
       </c>
       <c r="D8">
-        <v>0.75490000000000002</v>
+        <v>0.76529999999999998</v>
       </c>
       <c r="E8">
-        <v>0.75570000000000004</v>
+        <v>0.76570000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -2814,16 +2814,16 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0.87529999999999997</v>
+        <v>0.82840000000000003</v>
       </c>
       <c r="C9">
-        <v>0.75419999999999998</v>
+        <v>0.77849999999999997</v>
       </c>
       <c r="D9">
-        <v>0.7399</v>
+        <v>0.73040000000000005</v>
       </c>
       <c r="E9">
-        <v>0.74070000000000003</v>
+        <v>0.73050000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -2831,16 +2831,16 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>0.87529999999999997</v>
+        <v>0.85729999999999995</v>
       </c>
       <c r="C10">
-        <v>0.75370000000000004</v>
+        <v>0.78090000000000004</v>
       </c>
       <c r="D10">
-        <v>0.73950000000000005</v>
+        <v>0.74990000000000001</v>
       </c>
       <c r="E10">
-        <v>0.74029999999999996</v>
+        <v>0.75029999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -2848,16 +2848,16 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>0.90759999999999996</v>
+        <v>0.88970000000000005</v>
       </c>
       <c r="C11">
-        <v>0.76219999999999999</v>
+        <v>0.78910000000000002</v>
       </c>
       <c r="D11">
-        <v>0.7661</v>
+        <v>0.77629999999999999</v>
       </c>
       <c r="E11">
-        <v>0.7671</v>
+        <v>0.77680000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -2865,16 +2865,16 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>0.92420000000000002</v>
+        <v>0.90559999999999996</v>
       </c>
       <c r="C12">
-        <v>0.75460000000000005</v>
+        <v>0.78590000000000004</v>
       </c>
       <c r="D12">
-        <v>0.77010000000000001</v>
+        <v>0.78359999999999996</v>
       </c>
       <c r="E12">
-        <v>0.77149999999999996</v>
+        <v>0.7843</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="19.5" x14ac:dyDescent="0.6">
@@ -2904,16 +2904,16 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <v>0.61270000000000002</v>
+        <v>0.56030000000000002</v>
       </c>
       <c r="C16">
-        <v>0.75600000000000001</v>
+        <v>0.78549999999999998</v>
       </c>
       <c r="D16">
-        <v>0.58330000000000004</v>
+        <v>0.57079999999999997</v>
       </c>
       <c r="E16">
-        <v>0.58489999999999998</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -2921,16 +2921,16 @@
         <v>2</v>
       </c>
       <c r="B17">
-        <v>0.7298</v>
+        <v>0.71189999999999998</v>
       </c>
       <c r="C17">
-        <v>0.77580000000000005</v>
+        <v>0.79890000000000005</v>
       </c>
       <c r="D17">
-        <v>0.66839999999999999</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="E17">
-        <v>0.66849999999999998</v>
+        <v>0.67449999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
@@ -2938,16 +2938,16 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>0.80010000000000003</v>
+        <v>0.79259999999999997</v>
       </c>
       <c r="C18">
-        <v>0.79849999999999999</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="D18">
-        <v>0.72799999999999998</v>
+        <v>0.74260000000000004</v>
       </c>
       <c r="E18">
-        <v>0.72799999999999998</v>
+        <v>0.74270000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
@@ -2955,16 +2955,16 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>0.89319999999999999</v>
+        <v>0.90349999999999997</v>
       </c>
       <c r="C19">
-        <v>0.77049999999999996</v>
+        <v>0.80330000000000001</v>
       </c>
       <c r="D19">
-        <v>0.76380000000000003</v>
+        <v>0.79579999999999995</v>
       </c>
       <c r="E19">
-        <v>0.76459999999999995</v>
+        <v>0.79630000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -2972,16 +2972,16 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <v>0.86699999999999999</v>
+        <v>0.84909999999999997</v>
       </c>
       <c r="C20">
-        <v>0.77749999999999997</v>
+        <v>0.80420000000000003</v>
       </c>
       <c r="D20">
-        <v>0.75319999999999998</v>
+        <v>0.76249999999999996</v>
       </c>
       <c r="E20">
-        <v>0.75370000000000004</v>
+        <v>0.76270000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
@@ -2989,16 +2989,16 @@
         <v>6</v>
       </c>
       <c r="B21">
-        <v>0.86699999999999999</v>
+        <v>0.84909999999999997</v>
       </c>
       <c r="C21">
-        <v>0.77649999999999997</v>
+        <v>0.7923</v>
       </c>
       <c r="D21">
-        <v>0.75249999999999995</v>
+        <v>0.75360000000000005</v>
       </c>
       <c r="E21">
-        <v>0.752</v>
+        <v>0.75370000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
@@ -3009,13 +3009,13 @@
         <v>0.88149999999999995</v>
       </c>
       <c r="C22">
-        <v>0.77139999999999997</v>
+        <v>0.79890000000000005</v>
       </c>
       <c r="D22">
-        <v>0.75729999999999997</v>
+        <v>0.77859999999999996</v>
       </c>
       <c r="E22">
-        <v>0.75800000000000001</v>
+        <v>0.77900000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -3026,13 +3026,13 @@
         <v>0.89459999999999995</v>
       </c>
       <c r="C23">
-        <v>0.76800000000000002</v>
+        <v>0.78859999999999997</v>
       </c>
       <c r="D23">
-        <v>0.76270000000000004</v>
+        <v>0.77880000000000005</v>
       </c>
       <c r="E23">
-        <v>0.76349999999999996</v>
+        <v>0.77939999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
@@ -3040,15 +3040,267 @@
         <v>9</v>
       </c>
       <c r="B24">
+        <v>0.89590000000000003</v>
+      </c>
+      <c r="C24">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="D24">
+        <v>0.79079999999999995</v>
+      </c>
+      <c r="E24">
+        <v>0.79120000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B28">
+        <v>0.63129999999999997</v>
+      </c>
+      <c r="C28">
+        <v>0.76910000000000001</v>
+      </c>
+      <c r="D28">
+        <v>0.60370000000000001</v>
+      </c>
+      <c r="E28">
+        <v>0.60509999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>0.745</v>
+      </c>
+      <c r="C29">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="D29">
+        <v>0.67079999999999995</v>
+      </c>
+      <c r="E29">
+        <v>0.67090000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>0.83530000000000004</v>
+      </c>
+      <c r="C30">
+        <v>0.77490000000000003</v>
+      </c>
+      <c r="D30">
+        <v>0.73180000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0.73199999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <v>0.89039999999999997</v>
+      </c>
+      <c r="C31">
+        <v>0.75380000000000003</v>
+      </c>
+      <c r="D31">
+        <v>0.74880000000000002</v>
+      </c>
+      <c r="E31">
+        <v>0.74980000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>0.89039999999999997</v>
+      </c>
+      <c r="C32">
+        <v>0.76129999999999998</v>
+      </c>
+      <c r="D32">
+        <v>0.75490000000000002</v>
+      </c>
+      <c r="E32">
+        <v>0.75570000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B33">
+        <v>0.87529999999999997</v>
+      </c>
+      <c r="C33">
+        <v>0.75419999999999998</v>
+      </c>
+      <c r="D33">
+        <v>0.7399</v>
+      </c>
+      <c r="E33">
+        <v>0.74070000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <v>0.87529999999999997</v>
+      </c>
+      <c r="C34">
+        <v>0.75370000000000004</v>
+      </c>
+      <c r="D34">
+        <v>0.73950000000000005</v>
+      </c>
+      <c r="E34">
+        <v>0.74029999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B35">
+        <v>0.90759999999999996</v>
+      </c>
+      <c r="C35">
+        <v>0.76219999999999999</v>
+      </c>
+      <c r="D35">
+        <v>0.7661</v>
+      </c>
+      <c r="E35">
+        <v>0.7671</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B36">
+        <v>0.92420000000000002</v>
+      </c>
+      <c r="C36">
+        <v>0.75460000000000005</v>
+      </c>
+      <c r="D36">
+        <v>0.77010000000000001</v>
+      </c>
+      <c r="E36">
+        <v>0.77149999999999996</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B40">
+        <v>0.61270000000000002</v>
+      </c>
+      <c r="C40">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="D40">
+        <v>0.58330000000000004</v>
+      </c>
+      <c r="E40">
+        <v>0.58489999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B41">
+        <v>0.7298</v>
+      </c>
+      <c r="C41">
+        <v>0.77580000000000005</v>
+      </c>
+      <c r="D41">
+        <v>0.66839999999999999</v>
+      </c>
+      <c r="E41">
+        <v>0.66849999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B42">
+        <v>0.80010000000000003</v>
+      </c>
+      <c r="C42">
+        <v>0.79849999999999999</v>
+      </c>
+      <c r="D42">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="E42">
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B43">
+        <v>0.89319999999999999</v>
+      </c>
+      <c r="C43">
+        <v>0.77049999999999996</v>
+      </c>
+      <c r="D43">
+        <v>0.76380000000000003</v>
+      </c>
+      <c r="E43">
+        <v>0.76459999999999995</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B44">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="C44">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="D44">
+        <v>0.75319999999999998</v>
+      </c>
+      <c r="E44">
+        <v>0.75370000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B45">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="C45">
+        <v>0.77649999999999997</v>
+      </c>
+      <c r="D45">
+        <v>0.75249999999999995</v>
+      </c>
+      <c r="E45">
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B46">
+        <v>0.88149999999999995</v>
+      </c>
+      <c r="C46">
+        <v>0.77139999999999997</v>
+      </c>
+      <c r="D46">
+        <v>0.75729999999999997</v>
+      </c>
+      <c r="E46">
+        <v>0.75800000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B47">
+        <v>0.89459999999999995</v>
+      </c>
+      <c r="C47">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="D47">
+        <v>0.76270000000000004</v>
+      </c>
+      <c r="E47">
+        <v>0.76349999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B48">
         <v>0.89870000000000005</v>
       </c>
-      <c r="C24">
+      <c r="C48">
         <v>0.77849999999999997</v>
       </c>
-      <c r="D24">
+      <c r="D48">
         <v>0.77349999999999997</v>
       </c>
-      <c r="E24">
+      <c r="E48">
         <v>0.7742</v>
       </c>
     </row>

</xml_diff>